<commit_message>
Revision 01 for submission
</commit_message>
<xml_diff>
--- a/R_ice_camp/GE_IC_clarence_colors.xlsx
+++ b/R_ice_camp/GE_IC_clarence_colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarencesim/Documents/GitHub/SIM_GreenEdge_IceCamp/R_ice_camp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0102D594-F202-AB44-ADB9-C9B367F1DDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710BE665-0402-0640-AB85-7595EB48861E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="5" xr2:uid="{C82C6348-593F-2744-A17B-23CA1ACF9DB4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="3" xr2:uid="{C82C6348-593F-2744-A17B-23CA1ACF9DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="division" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="280">
   <si>
     <t>species</t>
   </si>
@@ -604,12 +604,6 @@
     <t>mediumseagreen</t>
   </si>
   <si>
-    <t>Pedinophyceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">palegreen1 </t>
-  </si>
-  <si>
     <t>Prasino-Clade-V</t>
   </si>
   <si>
@@ -884,6 +878,9 @@
   </si>
   <si>
     <t>#FCCDE5</t>
+  </si>
+  <si>
+    <t>Pavlovophyceae</t>
   </si>
 </sst>
 </file>
@@ -2545,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB275BB-30FF-9848-9078-6E31ED8BAB86}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="A1:D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -2615,28 +2612,28 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="18" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="22" t="s">
-        <v>188</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1">
       <c r="A6" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>189</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" thickBot="1">
@@ -2644,13 +2641,13 @@
         <v>29</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>192</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1">
@@ -2658,13 +2655,13 @@
         <v>29</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>195</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1">
@@ -2672,13 +2669,13 @@
         <v>29</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>198</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1">
@@ -2703,10 +2700,10 @@
         <v>36</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" thickBot="1">
@@ -2717,10 +2714,10 @@
         <v>18</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" thickBot="1">
@@ -2731,10 +2728,10 @@
         <v>61</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1">
@@ -2742,13 +2739,13 @@
         <v>41</v>
       </c>
       <c r="B14" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" thickBot="1">
@@ -2756,13 +2753,13 @@
         <v>41</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>210</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" thickBot="1">
@@ -2770,13 +2767,13 @@
         <v>41</v>
       </c>
       <c r="B16" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>213</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" thickBot="1">
@@ -2784,13 +2781,13 @@
         <v>41</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>216</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" thickBot="1">
@@ -2801,10 +2798,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" thickBot="1">
@@ -2812,13 +2809,13 @@
         <v>41</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" thickBot="1">
@@ -2826,13 +2823,13 @@
         <v>41</v>
       </c>
       <c r="B20" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" thickBot="1">
@@ -2840,13 +2837,13 @@
         <v>130</v>
       </c>
       <c r="B21" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>227</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" thickBot="1">
@@ -2854,13 +2851,13 @@
         <v>130</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>230</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2868,13 +2865,13 @@
         <v>35</v>
       </c>
       <c r="B23" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>233</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2882,27 +2879,27 @@
         <v>29</v>
       </c>
       <c r="B24" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>236</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="D25" s="26" t="s">
         <v>240</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2910,13 +2907,13 @@
         <v>41</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2924,13 +2921,13 @@
         <v>35</v>
       </c>
       <c r="B27" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>245</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2938,25 +2935,25 @@
         <v>110</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="18"/>
       <c r="B29" s="17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>102</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E29" s="1"/>
     </row>
@@ -2966,94 +2963,94 @@
         <v>174</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="18"/>
       <c r="B31" s="17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="18"/>
       <c r="B32" s="17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="18"/>
       <c r="B33" s="17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="18"/>
       <c r="B34" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="18"/>
       <c r="B35" s="17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="18"/>
       <c r="B36" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="18"/>
       <c r="B37" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D37" s="26" t="s">
         <v>266</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3062,22 +3059,22 @@
         <v>176</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="18"/>
       <c r="B39" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3086,58 +3083,58 @@
         <v>175</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="18"/>
       <c r="B41" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="18"/>
       <c r="B42" s="17" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="18"/>
       <c r="B43" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="18"/>
       <c r="B44" s="17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3222,7 +3219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDEB270-CEAB-104D-996D-855555300F9C}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3231,7 +3228,7 @@
     <col min="1" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="18" customFormat="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="27" t="s">
         <v>132</v>
       </c>
@@ -3242,7 +3239,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="18" customFormat="1">
+    <row r="2" spans="1:3">
       <c r="A2" s="25" t="s">
         <v>133</v>
       </c>
@@ -3253,7 +3250,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="18" customFormat="1">
+    <row r="3" spans="1:3">
       <c r="A3" s="18" t="s">
         <v>149</v>
       </c>
@@ -3264,7 +3261,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="18" customFormat="1">
+    <row r="4" spans="1:3">
       <c r="A4" s="25" t="s">
         <v>152</v>
       </c>
@@ -3275,7 +3272,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="18" customFormat="1">
+    <row r="5" spans="1:3">
       <c r="A5" s="25" t="s">
         <v>148</v>
       </c>
@@ -3286,7 +3283,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="18" customFormat="1">
+    <row r="6" spans="1:3">
       <c r="A6" s="25" t="s">
         <v>150</v>
       </c>
@@ -3297,7 +3294,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="18" customFormat="1">
+    <row r="7" spans="1:3">
       <c r="A7" s="25" t="s">
         <v>151</v>
       </c>
@@ -3308,7 +3305,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="18" customFormat="1">
+    <row r="8" spans="1:3">
       <c r="A8" s="25" t="s">
         <v>134</v>
       </c>
@@ -3319,7 +3316,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="18" customFormat="1">
+    <row r="9" spans="1:3">
       <c r="A9" s="25" t="s">
         <v>155</v>
       </c>

</xml_diff>